<commit_message>
Updated testing sheet with new tests
</commit_message>
<xml_diff>
--- a/Testing_Sheet.xlsx
+++ b/Testing_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fortn\OneDrive\Documents\Agile Project Work#\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0312969\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A246534-7C32-439B-B3E2-4B36E45716B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938B295A-79D3-4015-847A-E76765ED352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{CD12BE3F-3D8E-4689-A75D-33299C2705DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Testing</t>
   </si>
@@ -80,13 +80,31 @@
     <t>No Action Required</t>
   </si>
   <si>
-    <t xml:space="preserve">Both scripts worked as intended </t>
+    <t>Search script would not cancel when white is seen.</t>
+  </si>
+  <si>
+    <t>altered code after each rotation on the search added "Reuturn" script when sensors sees white during search</t>
+  </si>
+  <si>
+    <t>tested audio feedback</t>
+  </si>
+  <si>
+    <t>script failed with errors</t>
+  </si>
+  <si>
+    <t>did researcj to find out documentation was out of date. Used microsoft co-pilot to reaserch other scrips that may work and found one. Altered script until audio feedback worked.</t>
+  </si>
+  <si>
+    <t>Testing all code</t>
+  </si>
+  <si>
+    <t>All code worked as intended</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,14 +134,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{F5DFBAF1-B696-42A3-80E9-D32F4FE914E5}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -452,71 +478,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED373241-816E-463D-B448-C7B404E18776}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>